<commit_message>
Speicher -> Wirkungsgrad hinzugefügt
</commit_message>
<xml_diff>
--- a/Ergebnisse - Deutschland Vergleich.xlsx
+++ b/Ergebnisse - Deutschland Vergleich.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\OneDrive\Dokumente\SENCE\Semester 2_Projekte\Projekt 1_EWI_03_2022\EWI Einstiegsmodell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3307B365-E900-4A16-A873-DCAF36BE3DF7}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3236B194-0661-4BAC-819C-372D904351B8}"/>
   <bookViews>
     <workbookView xWindow="383" yWindow="458" windowWidth="28043" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -547,7 +547,7 @@
     <col min="3" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="18.5625" customWidth="1"/>
     <col min="19" max="19" width="18.125" customWidth="1"/>
-    <col min="20" max="20" width="10.875" customWidth="1"/>
+    <col min="20" max="20" width="12.1875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.5">

</xml_diff>